<commit_message>
Update na deliverables list
</commit_message>
<xml_diff>
--- a/I1/Current_Working_Directory/I1/Others/ABM-I1-DevilerablesAndRoles.xlsx
+++ b/I1/Current_Working_Directory/I1/Others/ABM-I1-DevilerablesAndRoles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Документи" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="89">
   <si>
     <t> Наименование</t>
   </si>
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,7 +645,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -661,9 +661,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office тема">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Оffice">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -701,7 +701,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Оffice">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -773,7 +773,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Оffice">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,7 +1613,9 @@
       <c r="D20" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="18" t="s">
+        <v>14</v>
+      </c>
       <c r="F20" s="18" t="s">
         <v>7</v>
       </c>
@@ -1715,13 +1717,13 @@
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="19" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>7</v>
@@ -1746,13 +1748,13 @@
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="19" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>7</v>
@@ -1777,16 +1779,16 @@
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="19" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K25" s="20" t="s">
         <v>65</v>
@@ -1808,16 +1810,16 @@
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="19" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K26" s="20" t="s">
         <v>66</v>
@@ -2029,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>